<commit_message>
Added async update for XML
</commit_message>
<xml_diff>
--- a/Currency_names.xlsx
+++ b/Currency_names.xlsx
@@ -2733,7 +2733,7 @@
   <dimension ref="A1:L187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2897,11 +2897,12 @@
         <v>355</v>
       </c>
       <c r="C15">
-        <v>1234</v>
+        <f>INDEX($K$15:$K$187,MATCH(A15,$L$15:$L$187,0))</f>
+        <v>64.349997999999999</v>
       </c>
       <c r="E15" t="str">
         <f>CONCATENATE($E$6,A15,$E$7,B15,$E$8,C15,$E$9)</f>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("AFN", "Afghan Afghani", 1234));</v>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("AFN", "Afghan Afghani", 64.349998));</v>
       </c>
       <c r="K15">
         <v>1174.295044</v>
@@ -2918,11 +2919,12 @@
         <v>180</v>
       </c>
       <c r="C16">
-        <v>1234</v>
+        <f t="shared" ref="C16:C79" si="0">INDEX($K$15:$K$187,MATCH(A16,$L$15:$L$187,0))</f>
+        <v>122.05950199999999</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" ref="E16:E79" si="0">CONCATENATE($E$6,A16,$E$7,B16,$E$8,C16,$E$9)</f>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ALL", "Albanian Lek", 1234));</v>
+        <f t="shared" ref="E16:E79" si="1">CONCATENATE($E$6,A16,$E$7,B16,$E$8,C16,$E$9)</f>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ALL", "Albanian Lek", 122.059502));</v>
       </c>
       <c r="K16">
         <v>6.5989000000000006E-2</v>
@@ -2939,11 +2941,12 @@
         <v>181</v>
       </c>
       <c r="C17">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>105.470001</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("DZD", "Algerian Dinar", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("DZD", "Algerian Dinar", 105.470001));</v>
       </c>
       <c r="K17">
         <v>22475</v>
@@ -2960,11 +2963,12 @@
         <v>182</v>
       </c>
       <c r="C18">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>135.29499799999999</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("AOA", "Angolan Kwanza", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("AOA", "Angolan Kwanza", 135.294998));</v>
       </c>
       <c r="K18">
         <v>6.9</v>
@@ -2981,11 +2985,12 @@
         <v>183</v>
       </c>
       <c r="C19">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>9.3998000000000008</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ARS", "Argentine Peso", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ARS", "Argentine Peso", 9.3998));</v>
       </c>
       <c r="K19">
         <v>7.9825999999999997</v>
@@ -3002,11 +3007,12 @@
         <v>184</v>
       </c>
       <c r="C20">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>481.73998999999998</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("AMD", "Armenian Dram", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("AMD", "Armenian Dram", 481.73999));</v>
       </c>
       <c r="K20">
         <v>77.822952000000001</v>
@@ -3023,11 +3029,12 @@
         <v>185</v>
       </c>
       <c r="C21">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>1.79</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("AWG", "Aruban Florin", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("AWG", "Aruban Florin", 1.79));</v>
       </c>
       <c r="K21">
         <v>19.899999999999999</v>
@@ -3044,11 +3051,12 @@
         <v>173</v>
       </c>
       <c r="C22">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>1.390144</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("AUD", "Australian Dollar", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("AUD", "Australian Dollar", 1.390144));</v>
       </c>
       <c r="K22">
         <v>6.35</v>
@@ -3065,11 +3073,12 @@
         <v>371</v>
       </c>
       <c r="C23">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>1.0568</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("AZN", "Azerbaijani Manat", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("AZN", "Azerbaijani Manat", 1.0568));</v>
       </c>
       <c r="K23">
         <v>2.4500000000000002</v>
@@ -3086,11 +3095,12 @@
         <v>187</v>
       </c>
       <c r="C24">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BSD", "Bahamian Dollar", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BSD", "Bahamian Dollar", 1));</v>
       </c>
       <c r="K24">
         <v>127.324997</v>
@@ -3107,11 +3117,12 @@
         <v>188</v>
       </c>
       <c r="C25">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>0.37740000000000001</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BHD", "Bahraini Dinar", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BHD", "Bahraini Dinar", 0.3774));</v>
       </c>
       <c r="K25">
         <v>17495</v>
@@ -3128,11 +3139,12 @@
         <v>189</v>
       </c>
       <c r="C26">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>77.822952000000001</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BDT", "Bangladeshi Taka", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BDT", "Bangladeshi Taka", 77.822952));</v>
       </c>
       <c r="K26">
         <v>35.647998999999999</v>
@@ -3149,11 +3161,12 @@
         <v>190</v>
       </c>
       <c r="C27">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BBD", "Barbados Dollar", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BBD", "Barbados Dollar", 2));</v>
       </c>
       <c r="K27">
         <v>2.81</v>
@@ -3170,11 +3183,12 @@
         <v>191</v>
       </c>
       <c r="C28">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>17495</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BYR", "Belarusian Ruble", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BYR", "Belarusian Ruble", 17495));</v>
       </c>
       <c r="K28">
         <v>1.9515499999999999</v>
@@ -3191,11 +3205,12 @@
         <v>192</v>
       </c>
       <c r="C29">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>1.9950000000000001</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BZD", "Belize Dollar", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BZD", "Belize Dollar", 1.995));</v>
       </c>
       <c r="K29">
         <v>118.5</v>
@@ -3212,11 +3227,12 @@
         <v>193</v>
       </c>
       <c r="C30">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BMD", "Bermudian Dollar", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BMD", "Bermudian Dollar", 1));</v>
       </c>
       <c r="K30">
         <v>6.6075499999999998</v>
@@ -3233,11 +3249,12 @@
         <v>379</v>
       </c>
       <c r="C31">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>65.764999000000003</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BTN", "Bhutanese Ngultrum", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BTN", "Bhutanese Ngultrum", 65.764999));</v>
       </c>
       <c r="K31">
         <v>3.3</v>
@@ -3254,11 +3271,12 @@
         <v>195</v>
       </c>
       <c r="C32">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>6.9</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BOB", "Bolivian Boliviano", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BOB", "Bolivian Boliviano", 6.9));</v>
       </c>
       <c r="K32">
         <v>10.247949999999999</v>
@@ -3275,11 +3293,12 @@
         <v>392</v>
       </c>
       <c r="C33">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>1.7315</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BAM", "Bosnia-Herzegovina Convertible Mark", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BAM", "Bosnia-Herzegovina Convertible Mark", 1.7315));</v>
       </c>
       <c r="K33">
         <v>8.1640499999999996</v>
@@ -3296,11 +3315,12 @@
         <v>197</v>
       </c>
       <c r="C34">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>10.247949999999999</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BWP", "Botswana Pula", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BWP", "Botswana Pula", 10.24795));</v>
       </c>
       <c r="K34">
         <v>35.450001</v>
@@ -3317,11 +3337,12 @@
         <v>198</v>
       </c>
       <c r="C35">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>3.9415</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BRL", "Brazilian Real", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BRL", "Brazilian Real", 3.9415));</v>
       </c>
       <c r="K35">
         <v>1.0568</v>
@@ -3338,11 +3359,12 @@
         <v>199</v>
       </c>
       <c r="C36">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>1.40215</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BND", "Brunei Dollar", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BND", "Brunei Dollar", 1.40215));</v>
       </c>
       <c r="K36">
         <v>65.870452999999998</v>
@@ -3359,11 +3381,12 @@
         <v>200</v>
       </c>
       <c r="C37">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>1.7321</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BGN", "Bulgarian Lev", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BGN", "Bulgarian Lev", 1.7321));</v>
       </c>
       <c r="K37">
         <v>3098.6000979999999</v>
@@ -3380,11 +3403,12 @@
         <v>397</v>
       </c>
       <c r="C38">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>1549</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BIF", "Burundian Franc", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("BIF", "Burundian Franc", 1549));</v>
       </c>
       <c r="K38">
         <v>1.32145</v>
@@ -3401,11 +3425,12 @@
         <v>205</v>
       </c>
       <c r="C39">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>4094.9499510000001</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KHR", "Cambodian Riel", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KHR", "Cambodian Riel", 4094.949951));</v>
       </c>
       <c r="K39">
         <v>580.724243</v>
@@ -3422,11 +3447,12 @@
         <v>207</v>
       </c>
       <c r="C40">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>97.049499999999995</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CVE", "Cape Verde Escudo", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CVE", "Cape Verde Escudo", 97.0495));</v>
       </c>
       <c r="K40">
         <v>1506.5</v>
@@ -3443,11 +3469,12 @@
         <v>208</v>
       </c>
       <c r="C41">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>0.82</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KYD", "Cayman Islands Dollar", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KYD", "Cayman Islands Dollar", 0.82));</v>
       </c>
       <c r="K41">
         <v>0.70874999999999999</v>
@@ -3464,11 +3491,12 @@
         <v>404</v>
       </c>
       <c r="C42">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>580.724243</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XAF", "Central African CFA", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XAF", "Central African CFA", 580.724243));</v>
       </c>
       <c r="K42">
         <v>14420.5</v>
@@ -3485,11 +3513,12 @@
         <v>204</v>
       </c>
       <c r="C43">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>105.64540100000001</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XPF", "CFP Franc", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XPF", "CFP Franc", 105.645401));</v>
       </c>
       <c r="K43">
         <v>0.69915400000000005</v>
@@ -3506,11 +3535,12 @@
         <v>209</v>
       </c>
       <c r="C44">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>678.55499299999997</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CLP", "Chilean Peso", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CLP", "Chilean Peso", 678.554993));</v>
       </c>
       <c r="K44">
         <v>1.390144</v>
@@ -3527,11 +3557,12 @@
         <v>353</v>
       </c>
       <c r="C45">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>2.46E-2</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CLF", "Chilean Unidad de Fomento", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CLF", "Chilean Unidad de Fomento", 0.0246));</v>
       </c>
       <c r="K45">
         <v>1282.400024</v>
@@ -3548,11 +3579,12 @@
         <v>352</v>
       </c>
       <c r="C46">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>6.3875500000000001</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CNH", "Chinese Offshore Yuan", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CNH", "Chinese Offshore Yuan", 6.38755));</v>
       </c>
       <c r="K46">
         <v>1.3649500000000001</v>
@@ -3569,11 +3601,12 @@
         <v>406</v>
       </c>
       <c r="C47">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>6.3702500000000004</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CNY", "Chinese Yuan", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CNY", "Chinese Yuan", 6.37025));</v>
       </c>
       <c r="K47">
         <v>13.3139</v>
@@ -3590,11 +3623,12 @@
         <v>211</v>
       </c>
       <c r="C48">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>2984.830078</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("COP", "Colombian Peso", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("COP", "Colombian Peso", 2984.830078));</v>
       </c>
       <c r="K48">
         <v>1188</v>
@@ -3611,11 +3645,12 @@
         <v>409</v>
       </c>
       <c r="C49">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>435.54321299999998</v>
       </c>
       <c r="E49" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KMF", "Comorian Franc", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KMF", "Comorian Franc", 435.543213));</v>
       </c>
       <c r="K49">
         <v>105.64540100000001</v>
@@ -3632,11 +3667,12 @@
         <v>213</v>
       </c>
       <c r="C50">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>927.5</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CDF", "Congolese Franc", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CDF", "Congolese Franc", 927.5));</v>
       </c>
       <c r="K50">
         <v>6.4005000000000001</v>
@@ -3653,11 +3689,12 @@
         <v>351</v>
       </c>
       <c r="C51">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>0.41946299999999997</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XCP", "Copper (lb)", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XCP", "Copper (lb)", 0.419463));</v>
       </c>
       <c r="K51">
         <v>1</v>
@@ -3674,11 +3711,12 @@
         <v>214</v>
       </c>
       <c r="C52">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>532.29998799999998</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CRC", "Costa Rican Colon", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CRC", "Costa Rican Colon", 532.299988));</v>
       </c>
       <c r="K52">
         <v>3650</v>
@@ -3695,11 +3733,12 @@
         <v>215</v>
       </c>
       <c r="C53">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>6.7590500000000002</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("HRK", "Croatian Kuna", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("HRK", "Croatian Kuna", 6.75905));</v>
       </c>
       <c r="K53">
         <v>199.04499799999999</v>
@@ -3716,11 +3755,12 @@
         <v>218</v>
       </c>
       <c r="C54">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CUP", "Cuban Peso", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CUP", "Cuban Peso", 1));</v>
       </c>
       <c r="K54">
         <v>2.8301500000000002</v>
@@ -3737,11 +3777,12 @@
         <v>419</v>
       </c>
       <c r="C55">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>0.51954999999999996</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CYP", "Cypriot Pound", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CYP", "Cypriot Pound", 0.51955));</v>
       </c>
       <c r="K55">
         <v>2.1749100000000001</v>
@@ -3758,11 +3799,12 @@
         <v>220</v>
       </c>
       <c r="C56">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>23.975000000000001</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CZK", "Czech Koruna", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("CZK", "Czech Koruna", 23.975));</v>
       </c>
       <c r="K56">
         <v>3.5</v>
@@ -3779,11 +3821,12 @@
         <v>221</v>
       </c>
       <c r="C57">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>6.6075499999999998</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("DKK", "Danish Krone", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("DKK", "Danish Krone", 6.60755));</v>
       </c>
       <c r="K57">
         <v>105.14949799999999</v>
@@ -3800,11 +3843,12 @@
         <v>709</v>
       </c>
       <c r="C58">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>1.7174499999999999</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("DEM", "Deutsche Mark (obsolete)", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("DEM", "Deutsche Mark (obsolete)", 1.71745));</v>
       </c>
       <c r="K58">
         <v>532.29998799999998</v>
@@ -3821,11 +3865,12 @@
         <v>432</v>
       </c>
       <c r="C59">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>176.99499499999999</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("DJF", "Djiboutian Franc", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("DJF", "Djiboutian Franc", 176.994995));</v>
       </c>
       <c r="K59">
         <v>43.169998</v>
@@ -3842,11 +3887,12 @@
         <v>435</v>
       </c>
       <c r="C60">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>45.209999000000003</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("DOP", "Dominican Peso", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("DOP", "Dominican Peso", 45.209999));</v>
       </c>
       <c r="K60">
         <v>188.78599500000001</v>
@@ -3863,11 +3909,12 @@
         <v>224</v>
       </c>
       <c r="C61">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>2.7</v>
       </c>
       <c r="E61" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XCD", "East Caribbean Dollar", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XCD", "East Caribbean Dollar", 2.7));</v>
       </c>
       <c r="K61">
         <v>1.79</v>
@@ -3884,11 +3931,12 @@
         <v>710</v>
       </c>
       <c r="C62">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>25000</v>
       </c>
       <c r="E62" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ECS", "Ecuadorian Sucre (obsolete)", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ECS", "Ecuadorian Sucre (obsolete)", 25000));</v>
       </c>
       <c r="K62">
         <v>10.003</v>
@@ -3905,11 +3953,12 @@
         <v>225</v>
       </c>
       <c r="C63">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>7.8304999999999998</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("EGP", "Egyptian Pound", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("EGP", "Egyptian Pound", 7.8305));</v>
       </c>
       <c r="K63">
         <v>3.9415</v>
@@ -3926,11 +3975,12 @@
         <v>441</v>
       </c>
       <c r="C64">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>8.7324999999999999</v>
       </c>
       <c r="E64" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SVC", "El Salvador Colon (obsolete)", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SVC", "El Salvador Colon (obsolete)", 8.7325));</v>
       </c>
       <c r="K64">
         <v>1</v>
@@ -3947,11 +3997,12 @@
         <v>347</v>
       </c>
       <c r="C65">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>15.28</v>
       </c>
       <c r="E65" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ERN", "Eritrean Nakfa", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ERN", "Eritrean Nakfa", 15.28));</v>
       </c>
       <c r="K65">
         <v>27.553801</v>
@@ -3968,11 +4019,12 @@
         <v>229</v>
       </c>
       <c r="C66">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>20.898001000000001</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ETB", "Ethiopian Birr", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ETB", "Ethiopian Birr", 20.898001));</v>
       </c>
       <c r="K66">
         <v>7249.9501950000003</v>
@@ -3989,11 +4041,12 @@
         <v>230</v>
       </c>
       <c r="C67">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>0.64849999999999997</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("FKP", "Falkland Islands Pound", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("FKP", "Falkland Islands Pound", 0.6485));</v>
       </c>
       <c r="K67">
         <v>1</v>
@@ -4010,11 +4063,12 @@
         <v>231</v>
       </c>
       <c r="C68">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>2.15795</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("FJD", "Fiji Dollar", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("FJD", "Fiji Dollar", 2.15795));</v>
       </c>
       <c r="K68">
         <v>4308</v>
@@ -4031,11 +4085,12 @@
         <v>707</v>
       </c>
       <c r="C69">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>5.7601000000000004</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("FRF", "French Franc (obsolete)", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("FRF", "French Franc (obsolete)", 5.7601));</v>
       </c>
       <c r="K69">
         <v>53.91</v>
@@ -4052,11 +4107,12 @@
         <v>232</v>
       </c>
       <c r="C70">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>38.93</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("GMD", "Gambian Dalasi", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("GMD", "Gambian Dalasi", 38.93));</v>
       </c>
       <c r="K70">
         <v>1549</v>
@@ -4073,11 +4129,12 @@
         <v>233</v>
       </c>
       <c r="C71">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>2.4500000000000002</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("GEL", "Georgian Lari", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("GEL", "Georgian Lari", 2.45));</v>
       </c>
       <c r="K71">
         <v>8129.9501950000003</v>
@@ -4094,11 +4151,12 @@
         <v>473</v>
       </c>
       <c r="C72">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>3.9</v>
       </c>
       <c r="E72" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("GHS", "Ghanaian Cedi", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("GHS", "Ghanaian Cedi", 3.9));</v>
       </c>
       <c r="K72">
         <v>0.37740000000000001</v>
@@ -4115,11 +4173,12 @@
         <v>235</v>
       </c>
       <c r="C73">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>0.64249999999999996</v>
       </c>
       <c r="E73" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("GIP", "Gibraltar Pound", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("GIP", "Gibraltar Pound", 0.6425));</v>
       </c>
       <c r="K73">
         <v>0.64249999999999996</v>
@@ -4136,11 +4195,12 @@
         <v>236</v>
       </c>
       <c r="C74">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>8.7900000000000001E-4</v>
       </c>
       <c r="E74" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XAU", "Gold (oz)", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XAU", "Gold (oz)", 0.000879));</v>
       </c>
       <c r="K74">
         <v>1.7321</v>
@@ -4157,11 +4217,12 @@
         <v>237</v>
       </c>
       <c r="C75">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>7.6544999999999996</v>
       </c>
       <c r="E75" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("GTQ", "Guatemalan Quetzal", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("GTQ", "Guatemalan Quetzal", 7.6545));</v>
       </c>
       <c r="K75">
         <v>1.4012</v>
@@ -4178,11 +4239,12 @@
         <v>482</v>
       </c>
       <c r="C76">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>7249.9501950000003</v>
       </c>
       <c r="E76" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("GNF", "Guinean Franc", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("GNF", "Guinean Franc", 7249.950195));</v>
       </c>
       <c r="K76">
         <v>6.3702500000000004</v>
@@ -4199,11 +4261,12 @@
         <v>239</v>
       </c>
       <c r="C77">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>207.21000699999999</v>
       </c>
       <c r="E77" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("GYD", "Guyanese Dollar", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("GYD", "Guyanese Dollar", 207.210007));</v>
       </c>
       <c r="K77">
         <v>0.88558700000000001</v>
@@ -4220,11 +4283,12 @@
         <v>240</v>
       </c>
       <c r="C78">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>51.737499</v>
       </c>
       <c r="E78" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("HTG", "Haitian Gourde", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("HTG", "Haitian Gourde", 51.737499));</v>
       </c>
       <c r="K78">
         <v>6.3381999999999996</v>
@@ -4241,11 +4305,12 @@
         <v>241</v>
       </c>
       <c r="C79">
-        <v>1234</v>
+        <f t="shared" si="0"/>
+        <v>21.949698999999999</v>
       </c>
       <c r="E79" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("HNL", "Honduran Lempira", 1234));</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("HNL", "Honduran Lempira", 21.949699));</v>
       </c>
       <c r="K79">
         <v>13.09995</v>
@@ -4262,11 +4327,12 @@
         <v>243</v>
       </c>
       <c r="C80">
-        <v>1234</v>
+        <f t="shared" ref="C80:C143" si="2">INDEX($K$15:$K$187,MATCH(A80,$L$15:$L$187,0))</f>
+        <v>275.36999500000002</v>
       </c>
       <c r="E80" t="str">
-        <f t="shared" ref="E80:E143" si="1">CONCATENATE($E$6,A80,$E$7,B80,$E$8,C80,$E$9)</f>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("HUF", "Hungarian Forint", 1234));</v>
+        <f t="shared" ref="E80:E143" si="3">CONCATENATE($E$6,A80,$E$7,B80,$E$8,C80,$E$9)</f>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("HUF", "Hungarian Forint", 275.369995));</v>
       </c>
       <c r="K80">
         <v>2</v>
@@ -4283,11 +4349,12 @@
         <v>487</v>
       </c>
       <c r="C81">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>127.324997</v>
       </c>
       <c r="E81" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ISK", "Icelandic Krona", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ISK", "Icelandic Krona", 127.324997));</v>
       </c>
       <c r="K81">
         <v>7.9715660000000002</v>
@@ -4304,11 +4371,12 @@
         <v>245</v>
       </c>
       <c r="C82">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>65.870452999999998</v>
       </c>
       <c r="E82" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("INR", "Indian Rupee", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("INR", "Indian Rupee", 65.870453));</v>
       </c>
       <c r="K82">
         <v>9.6715499999999999</v>
@@ -4325,11 +4393,12 @@
         <v>246</v>
       </c>
       <c r="C83">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>14420.5</v>
       </c>
       <c r="E83" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("IDR", "Indonesian Rupiah", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("IDR", "Indonesian Rupiah", 14420.5));</v>
       </c>
       <c r="K83">
         <v>7.6544999999999996</v>
@@ -4346,11 +4415,12 @@
         <v>247</v>
       </c>
       <c r="C84">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>29605</v>
       </c>
       <c r="E84" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("IRR", "Iranian Rial", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("IRR", "Iranian Rial", 29605));</v>
       </c>
       <c r="K84">
         <v>557.49499500000002</v>
@@ -4367,11 +4437,12 @@
         <v>248</v>
       </c>
       <c r="C85">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>1188</v>
       </c>
       <c r="E85" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("IQD", "Iraqi Dinar", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("IQD", "Iraqi Dinar", 1188));</v>
       </c>
       <c r="K85">
         <v>104.355003</v>
@@ -4388,11 +4459,12 @@
         <v>345</v>
       </c>
       <c r="C86">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>0.69915400000000005</v>
       </c>
       <c r="E86" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("IEP", "Irish Pound", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("IEP", "Irish Pound", 0.699154));</v>
       </c>
       <c r="K86">
         <v>1700.272217</v>
@@ -4409,11 +4481,12 @@
         <v>249</v>
       </c>
       <c r="C87">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>3.9344000000000001</v>
       </c>
       <c r="E87" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ILS", "Israeli New Shekel", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ILS", "Israeli New Shekel", 3.9344));</v>
       </c>
       <c r="K87">
         <v>3.19</v>
@@ -4430,11 +4503,12 @@
         <v>706</v>
       </c>
       <c r="C88">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>1700.272217</v>
       </c>
       <c r="E88" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ITL", "Italian Lira (obsolete)", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ITL", "Italian Lira (obsolete)", 1700.272217));</v>
       </c>
       <c r="K88">
         <v>3.6727500000000002</v>
@@ -4451,11 +4525,12 @@
         <v>250</v>
       </c>
       <c r="C89">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>118.5</v>
       </c>
       <c r="E89" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("JMD", "Jamaican Dollar", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("JMD", "Jamaican Dollar", 118.5));</v>
       </c>
       <c r="K89">
         <v>0.62055000000000005</v>
@@ -4472,11 +4547,12 @@
         <v>251</v>
       </c>
       <c r="C90">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>0.70899999999999996</v>
       </c>
       <c r="E90" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("JOD", "Jordanian Dinar", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("JOD", "Jordanian Dinar", 0.709));</v>
       </c>
       <c r="K90">
         <v>1.6379999999999999E-3</v>
@@ -4493,11 +4569,12 @@
         <v>504</v>
       </c>
       <c r="C91">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>275.90493800000002</v>
       </c>
       <c r="E91" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KZT", "Kazakhstani Tenge", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KZT", "Kazakhstani Tenge", 275.904938));</v>
       </c>
       <c r="K91">
         <v>21.799999</v>
@@ -4514,11 +4591,12 @@
         <v>253</v>
       </c>
       <c r="C92">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>105.14949799999999</v>
       </c>
       <c r="E92" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KES", "Kenyan Shilling", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KES", "Kenyan Shilling", 105.149498));</v>
       </c>
       <c r="K92">
         <v>5.7601000000000004</v>
@@ -4535,11 +4613,12 @@
         <v>254</v>
       </c>
       <c r="C93">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>0.30130000000000001</v>
       </c>
       <c r="E93" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KWD", "Kuwaiti Dinar", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KWD", "Kuwaiti Dinar", 0.3013));</v>
       </c>
       <c r="K93">
         <v>84.660004000000001</v>
@@ -4556,11 +4635,12 @@
         <v>255</v>
       </c>
       <c r="C94">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>70.493797000000001</v>
       </c>
       <c r="E94" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KGS", "Kyrgyzstanian Som", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KGS", "Kyrgyzstanian Som", 70.493797));</v>
       </c>
       <c r="K94">
         <v>13.315250000000001</v>
@@ -4577,11 +4657,12 @@
         <v>256</v>
       </c>
       <c r="C95">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>8129.9501950000003</v>
       </c>
       <c r="E95" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("LAK", "Lao Kip", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("LAK", "Lao Kip", 8129.950195));</v>
       </c>
       <c r="K95">
         <v>8.2580500000000008</v>
@@ -4598,11 +4679,12 @@
         <v>507</v>
       </c>
       <c r="C96">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>0.62055000000000005</v>
       </c>
       <c r="E96" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("LVL", "Latvian Lats (obsolete)", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("LVL", "Latvian Lats (obsolete)", 0.62055));</v>
       </c>
       <c r="K96">
         <v>3.8222499999999999</v>
@@ -4619,11 +4701,12 @@
         <v>258</v>
       </c>
       <c r="C97">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>1506.5</v>
       </c>
       <c r="E97" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("LBP", "Lebanese Pound", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("LBP", "Lebanese Pound", 1506.5));</v>
       </c>
       <c r="K97">
         <v>580.724243</v>
@@ -4640,11 +4723,12 @@
         <v>259</v>
       </c>
       <c r="C98">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>13.315250000000001</v>
       </c>
       <c r="E98" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("LSL", "Lesotho Loti", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("LSL", "Lesotho Loti", 13.31525));</v>
       </c>
       <c r="K98">
         <v>2984.830078</v>
@@ -4661,11 +4745,12 @@
         <v>260</v>
       </c>
       <c r="C99">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>84.660004000000001</v>
       </c>
       <c r="E99" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("LRD", "Liberian Dollar", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("LRD", "Liberian Dollar", 84.660004));</v>
       </c>
       <c r="K99">
         <v>927.5</v>
@@ -4682,11 +4767,12 @@
         <v>261</v>
       </c>
       <c r="C100">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>1.3649500000000001</v>
       </c>
       <c r="E100" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("LYD", "Libyan Dinar", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("LYD", "Libyan Dinar", 1.36495));</v>
       </c>
       <c r="K100">
         <v>1</v>
@@ -4703,11 +4789,12 @@
         <v>262</v>
       </c>
       <c r="C101">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>3.0487000000000002</v>
       </c>
       <c r="E101" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("LTL", "Lithuanian Litas", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("LTL", "Lithuanian Litas", 3.0487));</v>
       </c>
       <c r="K101">
         <v>2169.1999510000001</v>
@@ -4724,11 +4811,12 @@
         <v>263</v>
       </c>
       <c r="C102">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>7.9825999999999997</v>
       </c>
       <c r="E102" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MOP", "Macau Pataca", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MOP", "Macau Pataca", 7.9826));</v>
       </c>
       <c r="K102">
         <v>3.9</v>
@@ -4745,11 +4833,12 @@
         <v>264</v>
       </c>
       <c r="C103">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>53.91</v>
       </c>
       <c r="E103" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MKD", "Macedonian Denar", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MKD", "Macedonian Denar", 53.91));</v>
       </c>
       <c r="K103">
         <v>105.22399900000001</v>
@@ -4766,11 +4855,12 @@
         <v>265</v>
       </c>
       <c r="C104">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>3098.6000979999999</v>
       </c>
       <c r="E104" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MGA", "Malagasy Ariary", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MGA", "Malagasy Ariary", 3098.600098));</v>
       </c>
       <c r="K104">
         <v>322.35501099999999</v>
@@ -4787,11 +4877,12 @@
         <v>519</v>
       </c>
       <c r="C105">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>557.49499500000002</v>
       </c>
       <c r="E105" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MWK", "Malawian Kwacha", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MWK", "Malawian Kwacha", 557.494995));</v>
       </c>
       <c r="K105">
         <v>639.95001200000002</v>
@@ -4808,11 +4899,12 @@
         <v>267</v>
       </c>
       <c r="C106">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>4.2264999999999997</v>
       </c>
       <c r="E106" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MYR", "Malaysian Ringgit", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MYR", "Malaysian Ringgit", 4.2265));</v>
       </c>
       <c r="K106">
         <v>105.470001</v>
@@ -4829,11 +4921,12 @@
         <v>703</v>
       </c>
       <c r="C107">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>15.34</v>
       </c>
       <c r="E107" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MVR", "Maldivian Rufiyaa", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MVR", "Maldivian Rufiyaa", 15.34));</v>
       </c>
       <c r="K107">
         <v>0.64849999999999997</v>
@@ -4850,11 +4943,12 @@
         <v>271</v>
       </c>
       <c r="C108">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>290</v>
       </c>
       <c r="E108" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MRO", "Mauritanian Ouguiya", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MRO", "Mauritanian Ouguiya", 290));</v>
       </c>
       <c r="K108">
         <v>140.490005</v>
@@ -4871,11 +4965,12 @@
         <v>527</v>
       </c>
       <c r="C109">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>35.450001</v>
       </c>
       <c r="E109" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MUR", "Mauritian Rupee", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MUR", "Mauritian Rupee", 35.450001));</v>
       </c>
       <c r="K109">
         <v>119.985001</v>
@@ -4892,11 +4987,12 @@
         <v>273</v>
       </c>
       <c r="C110">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>16.622399999999999</v>
       </c>
       <c r="E110" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MXN", "Mexican Peso", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MXN", "Mexican Peso", 16.6224));</v>
       </c>
       <c r="K110">
         <v>0.96924999999999994</v>
@@ -4913,11 +5009,12 @@
         <v>343</v>
       </c>
       <c r="C111">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>2.81</v>
       </c>
       <c r="E111" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MXV", "Mexican Unidad de Inversion", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MXV", "Mexican Unidad de Inversion", 2.81));</v>
       </c>
       <c r="K111">
         <v>0.82</v>
@@ -4934,11 +5031,12 @@
         <v>274</v>
       </c>
       <c r="C112">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>19.899999999999999</v>
       </c>
       <c r="E112" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MDL", "Moldovan Leu", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MDL", "Moldovan Leu", 19.9));</v>
       </c>
       <c r="K112">
         <v>678.55499299999997</v>
@@ -4955,11 +5053,12 @@
         <v>275</v>
       </c>
       <c r="C113">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>1990.5</v>
       </c>
       <c r="E113" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MNT", "Mongolian Tugrik", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MNT", "Mongolian Tugrik", 1990.5));</v>
       </c>
       <c r="K113">
         <v>29605</v>
@@ -4976,11 +5075,12 @@
         <v>276</v>
       </c>
       <c r="C114">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>9.6715499999999999</v>
       </c>
       <c r="E114" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MAD", "Moroccan Dirham", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MAD", "Moroccan Dirham", 9.67155));</v>
       </c>
       <c r="K114">
         <v>64.349997999999999</v>
@@ -4997,11 +5097,12 @@
         <v>702</v>
       </c>
       <c r="C115">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>43.169998</v>
       </c>
       <c r="E115" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MZN", "Mozambican Metical", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MZN", "Mozambican Metical", 43.169998));</v>
       </c>
       <c r="K115">
         <v>176.99499499999999</v>
@@ -5018,11 +5119,12 @@
         <v>278</v>
       </c>
       <c r="C116">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>1282.400024</v>
       </c>
       <c r="E116" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MMK", "Myanmar Kyat", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("MMK", "Myanmar Kyat", 1282.400024));</v>
       </c>
       <c r="K116">
         <v>8.7324999999999999</v>
@@ -5039,11 +5141,12 @@
         <v>544</v>
       </c>
       <c r="C117">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>13.315250000000001</v>
       </c>
       <c r="E117" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("NAD", "Namibian Dollar", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("NAD", "Namibian Dollar", 13.31525));</v>
       </c>
       <c r="K117">
         <v>3.7231000000000001</v>
@@ -5060,11 +5163,12 @@
         <v>281</v>
       </c>
       <c r="C118">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>105.22399900000001</v>
       </c>
       <c r="E118" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("NPR", "Nepalese Rupee", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("NPR", "Nepalese Rupee", 105.223999));</v>
       </c>
       <c r="K118">
         <v>5474.6850590000004</v>
@@ -5081,11 +5185,12 @@
         <v>549</v>
       </c>
       <c r="C119">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>1.79</v>
       </c>
       <c r="E119" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ANG", "Netherlands Antillean Guilder", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ANG", "Netherlands Antillean Guilder", 1.79));</v>
       </c>
       <c r="K119">
         <v>15.28</v>
@@ -5102,11 +5207,12 @@
         <v>554</v>
       </c>
       <c r="C120">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>32.395000000000003</v>
       </c>
       <c r="E120" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("TWD", "New Taiwan Dollar", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("TWD", "New Taiwan Dollar", 32.395));</v>
       </c>
       <c r="K120">
         <v>20.898001000000001</v>
@@ -5123,11 +5229,12 @@
         <v>282</v>
       </c>
       <c r="C121">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>1.5634410000000001</v>
       </c>
       <c r="E121" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("NZD", "New Zealand Dollar", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("NZD", "New Zealand Dollar", 1.563441));</v>
       </c>
       <c r="K121">
         <v>3.9344000000000001</v>
@@ -5144,11 +5251,12 @@
         <v>283</v>
       </c>
       <c r="C122">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>27.553801</v>
       </c>
       <c r="E122" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("NIO", "Nicaraguan Cordoba Oro", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("NIO", "Nicaraguan Cordoba Oro", 27.553801));</v>
       </c>
       <c r="K122">
         <v>32.395000000000003</v>
@@ -5165,11 +5273,12 @@
         <v>284</v>
       </c>
       <c r="C123">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>199.04499799999999</v>
       </c>
       <c r="E123" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("NGN", "Nigerian Naira", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("NGN", "Nigerian Naira", 199.044998));</v>
       </c>
       <c r="K123">
         <v>900</v>
@@ -5186,11 +5295,12 @@
         <v>285</v>
       </c>
       <c r="C124">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>900</v>
       </c>
       <c r="E124" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KPW", "North Korean Won", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KPW", "North Korean Won", 900));</v>
       </c>
       <c r="K124">
         <v>216.48675499999999</v>
@@ -5207,11 +5317,12 @@
         <v>561</v>
       </c>
       <c r="C125">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>8.1640499999999996</v>
       </c>
       <c r="E125" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("NOK", "Norwegian Krone", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("NOK", "Norwegian Krone", 8.16405));</v>
       </c>
       <c r="K125">
         <v>0.64249999999999996</v>
@@ -5228,11 +5339,12 @@
         <v>287</v>
       </c>
       <c r="C126">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>0.38505</v>
       </c>
       <c r="E126" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("OMR", "Omani Rial", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("OMR", "Omani Rial", 0.38505));</v>
       </c>
       <c r="K126">
         <v>1.40215</v>
@@ -5249,11 +5361,12 @@
         <v>288</v>
       </c>
       <c r="C127">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>104.355003</v>
       </c>
       <c r="E127" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("PKR", "Pakistan Rupee", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("PKR", "Pakistan Rupee", 104.355003));</v>
       </c>
       <c r="K127">
         <v>21.949698999999999</v>
@@ -5270,11 +5383,12 @@
         <v>349</v>
       </c>
       <c r="C128">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>1.6379999999999999E-3</v>
       </c>
       <c r="E128" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XPD", "Palladium (oz)", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XPD", "Palladium (oz)", 0.001638));</v>
       </c>
       <c r="K128">
         <v>23.975000000000001</v>
@@ -5291,11 +5405,12 @@
         <v>289</v>
       </c>
       <c r="C129">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="E129" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("PAB", "Panamanian Balboa", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("PAB", "Panamanian Balboa", 1));</v>
       </c>
       <c r="K129">
         <v>275.36999500000002</v>
@@ -5312,11 +5427,12 @@
         <v>290</v>
       </c>
       <c r="C130">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>2.8301500000000002</v>
       </c>
       <c r="E130" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("PGK", "Papua New Guinea Kina", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("PGK", "Papua New Guinea Kina", 2.83015));</v>
       </c>
       <c r="K130">
         <v>1.9950000000000001</v>
@@ -5333,11 +5449,12 @@
         <v>291</v>
       </c>
       <c r="C131">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>5474.6850590000004</v>
       </c>
       <c r="E131" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("PYG", "Paraguay Guarani", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("PYG", "Paraguay Guarani", 5474.685059));</v>
       </c>
       <c r="K131">
         <v>1.7174499999999999</v>
@@ -5354,11 +5471,12 @@
         <v>292</v>
       </c>
       <c r="C132">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>3.19</v>
       </c>
       <c r="E132" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("PEN", "Peruvian Nuevo Sol", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("PEN", "Peruvian Nuevo Sol", 3.19));</v>
       </c>
       <c r="K132">
         <v>0.70899999999999996</v>
@@ -5375,11 +5493,12 @@
         <v>293</v>
       </c>
       <c r="C133">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>46.512501</v>
       </c>
       <c r="E133" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("PHP", "Philippine Peso", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("PHP", "Philippine Peso", 46.512501));</v>
       </c>
       <c r="K133">
         <v>732.080017</v>
@@ -5396,11 +5515,12 @@
         <v>348</v>
       </c>
       <c r="C134">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>1.016E-3</v>
       </c>
       <c r="E134" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XPT", "Platinum (oz)", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XPT", "Platinum (oz)", 0.001016));</v>
       </c>
       <c r="K134">
         <v>3.0487000000000002</v>
@@ -5417,11 +5537,12 @@
         <v>294</v>
       </c>
       <c r="C135">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>3.7231000000000001</v>
       </c>
       <c r="E135" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("PLN", "Polish Zloty", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("PLN", "Polish Zloty", 3.7231));</v>
       </c>
       <c r="K135">
         <v>66.499495999999994</v>
@@ -5438,11 +5559,12 @@
         <v>613</v>
       </c>
       <c r="C136">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>3.6438000000000001</v>
       </c>
       <c r="E136" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("QAR", "Qatari Riyal", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("QAR", "Qatari Riyal", 3.6438));</v>
       </c>
       <c r="K136">
         <v>106.220001</v>
@@ -5459,11 +5581,12 @@
         <v>622</v>
       </c>
       <c r="C137">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>3.8222499999999999</v>
       </c>
       <c r="E137" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("RON", "Romanian Leu", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("RON", "Romanian Leu", 3.82225));</v>
       </c>
       <c r="K137">
         <v>2.658703</v>
@@ -5480,11 +5603,12 @@
         <v>623</v>
       </c>
       <c r="C138">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>66.499495999999994</v>
       </c>
       <c r="E138" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("RUB", "Russian Ruble", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("RUB", "Russian Ruble", 66.499496));</v>
       </c>
       <c r="K138">
         <v>1.016E-3</v>
@@ -5501,11 +5625,12 @@
         <v>298</v>
       </c>
       <c r="C139">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>732.080017</v>
       </c>
       <c r="E139" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("RWF", "Rwandan Franc", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("RWF", "Rwandan Franc", 732.080017));</v>
       </c>
       <c r="K139">
         <v>13.315250000000001</v>
@@ -5522,11 +5647,12 @@
         <v>299</v>
       </c>
       <c r="C140">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>2.658703</v>
       </c>
       <c r="E140" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("WST", "Samoan Tala", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("WST", "Samoan Tala", 2.658703));</v>
       </c>
       <c r="K140">
         <v>1</v>
@@ -5543,11 +5669,12 @@
         <v>626</v>
       </c>
       <c r="C141">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>21495</v>
       </c>
       <c r="E141" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("STD", "Sao Tome Dobra", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("STD", "Sao Tome Dobra", 21495));</v>
       </c>
       <c r="K141">
         <v>45.209999000000003</v>
@@ -5564,11 +5691,12 @@
         <v>301</v>
       </c>
       <c r="C142">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>3.7500499999999999</v>
       </c>
       <c r="E142" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SAR", "Saudi Riyal", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SAR", "Saudi Riyal", 3.75005));</v>
       </c>
       <c r="K142">
         <v>122.05950199999999</v>
@@ -5585,11 +5713,12 @@
         <v>302</v>
       </c>
       <c r="C143">
-        <v>1234</v>
+        <f t="shared" si="2"/>
+        <v>106.220001</v>
       </c>
       <c r="E143" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("RSD", "Serbian Dinar", 1234));</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("RSD", "Serbian Dinar", 106.220001));</v>
       </c>
       <c r="K143">
         <v>51.737499</v>
@@ -5606,11 +5735,12 @@
         <v>303</v>
       </c>
       <c r="C144">
-        <v>1234</v>
+        <f t="shared" ref="C144:C180" si="4">INDEX($K$15:$K$187,MATCH(A144,$L$15:$L$187,0))</f>
+        <v>13.09995</v>
       </c>
       <c r="E144" t="str">
-        <f t="shared" ref="E144:E180" si="2">CONCATENATE($E$6,A144,$E$7,B144,$E$8,C144,$E$9)</f>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SCR", "Seychelles Rupee", 1234));</v>
+        <f t="shared" ref="E144:E180" si="5">CONCATENATE($E$6,A144,$E$7,B144,$E$8,C144,$E$9)</f>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SCR", "Seychelles Rupee", 13.09995));</v>
       </c>
       <c r="K144">
         <v>481.73998999999998</v>
@@ -5627,11 +5757,12 @@
         <v>634</v>
       </c>
       <c r="C145">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>4308</v>
       </c>
       <c r="E145" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SLL", "Sierra Leonean Leone", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SLL", "Sierra Leonean Leone", 4308));</v>
       </c>
       <c r="K145">
         <v>435.54321299999998</v>
@@ -5648,11 +5779,12 @@
         <v>305</v>
       </c>
       <c r="C146">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>6.5989000000000006E-2</v>
       </c>
       <c r="E146" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XAG", "Silver (oz)", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XAG", "Silver (oz)", 0.065989));</v>
       </c>
       <c r="K146">
         <v>290</v>
@@ -5669,11 +5801,12 @@
         <v>306</v>
       </c>
       <c r="C147">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>1.4012</v>
       </c>
       <c r="E147" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SGD", "Singapore Dollar", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SGD", "Singapore Dollar", 1.4012));</v>
       </c>
       <c r="K147">
         <v>6.7590500000000002</v>
@@ -5690,11 +5823,12 @@
         <v>638</v>
       </c>
       <c r="C148">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>216.48675499999999</v>
       </c>
       <c r="E148" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SIT", "Slovenian Tolar (obsolete)", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SIT", "Slovenian Tolar (obsolete)", 216.486755));</v>
       </c>
       <c r="K148">
         <v>25000</v>
@@ -5711,11 +5845,12 @@
         <v>310</v>
       </c>
       <c r="C149">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>7.9715660000000002</v>
       </c>
       <c r="E149" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SBD", "Solomon Islands Dollar", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SBD", "Solomon Islands Dollar", 7.971566));</v>
       </c>
       <c r="K149">
         <v>4094.9499510000001</v>
@@ -5732,11 +5867,12 @@
         <v>311</v>
       </c>
       <c r="C150">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>639.95001200000002</v>
       </c>
       <c r="E150" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SOS", "Somali Shilling", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SOS", "Somali Shilling", 639.950012));</v>
       </c>
       <c r="K150">
         <v>46.512501</v>
@@ -5753,11 +5889,12 @@
         <v>312</v>
       </c>
       <c r="C151">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>13.3139</v>
       </c>
       <c r="E151" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ZAR", "South African Rand", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ZAR", "South African Rand", 13.3139));</v>
       </c>
       <c r="K151">
         <v>0.51954999999999996</v>
@@ -5774,11 +5911,12 @@
         <v>313</v>
       </c>
       <c r="C152">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>1174.295044</v>
       </c>
       <c r="E152" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KRW", "South-Korean Won", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("KRW", "South-Korean Won", 1174.295044));</v>
       </c>
       <c r="K152">
         <v>0.30130000000000001</v>
@@ -5795,11 +5933,12 @@
         <v>344</v>
       </c>
       <c r="C153">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>0.70874999999999999</v>
       </c>
       <c r="E153" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XDR", "Special Drawing Rights", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XDR", "Special Drawing Rights", 0.70875));</v>
       </c>
       <c r="K153">
         <v>2.7</v>
@@ -5816,11 +5955,12 @@
         <v>647</v>
       </c>
       <c r="C154">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>140.490005</v>
       </c>
       <c r="E154" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("LKR", "Sri Lankan Rupee", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("LKR", "Sri Lankan Rupee", 140.490005));</v>
       </c>
       <c r="K154">
         <v>0.41946299999999997</v>
@@ -5837,11 +5977,12 @@
         <v>315</v>
       </c>
       <c r="C155">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>0.64249999999999996</v>
       </c>
       <c r="E155" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SHP", "St Helena Pound", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SHP", "St Helena Pound", 0.6425));</v>
       </c>
       <c r="K155">
         <v>6.3875500000000001</v>
@@ -5858,11 +5999,12 @@
         <v>316</v>
       </c>
       <c r="C156">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>6.09</v>
       </c>
       <c r="E156" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SDG", "Sudanese Pound", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SDG", "Sudanese Pound", 6.09));</v>
       </c>
       <c r="K156">
         <v>6.09</v>
@@ -5879,11 +6021,12 @@
         <v>317</v>
       </c>
       <c r="C157">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>3.3</v>
       </c>
       <c r="E157" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SRD", "Suriname Dollar", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SRD", "Suriname Dollar", 3.3));</v>
       </c>
       <c r="K157">
         <v>2.46E-2</v>
@@ -5900,11 +6043,12 @@
         <v>656</v>
       </c>
       <c r="C158">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>13.315250000000001</v>
       </c>
       <c r="E158" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SZL", "Swazi Lilangeni", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SZL", "Swazi Lilangeni", 13.31525));</v>
       </c>
       <c r="K158">
         <v>275.90493800000002</v>
@@ -5921,11 +6065,12 @@
         <v>319</v>
       </c>
       <c r="C159">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>8.2580500000000008</v>
       </c>
       <c r="E159" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SEK", "Swedish Krona", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SEK", "Swedish Krona", 8.25805));</v>
       </c>
       <c r="K159">
         <v>3.0063499999999999</v>
@@ -5942,11 +6087,12 @@
         <v>320</v>
       </c>
       <c r="C160">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>188.78599500000001</v>
       </c>
       <c r="E160" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SYP", "Syrian Pound", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("SYP", "Syrian Pound", 188.785995));</v>
       </c>
       <c r="K160">
         <v>2.15795</v>
@@ -5963,11 +6109,12 @@
         <v>346</v>
       </c>
       <c r="C161">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>6.4005000000000001</v>
       </c>
       <c r="E161" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("TJS", "Tajikistan Somoni", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("TJS", "Tajikistan Somoni", 6.4005));</v>
       </c>
       <c r="K161">
         <v>1.5634410000000001</v>
@@ -5984,11 +6131,12 @@
         <v>322</v>
       </c>
       <c r="C162">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>2169.1999510000001</v>
       </c>
       <c r="E162" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("TZS", "Tanzanian Shilling", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("TZS", "Tanzanian Shilling", 2169.199951));</v>
       </c>
       <c r="K162">
         <v>1.7315</v>
@@ -6005,11 +6153,12 @@
         <v>323</v>
       </c>
       <c r="C163">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>35.647998999999999</v>
       </c>
       <c r="E163" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("THB", "Thai Baht", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("THB", "Thai Baht", 35.647999));</v>
       </c>
       <c r="K163">
         <v>65.764999000000003</v>
@@ -6026,11 +6175,12 @@
         <v>324</v>
       </c>
       <c r="C164">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>2.1749100000000001</v>
       </c>
       <c r="E164" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("TOP", "Tonga Pa'anga", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("TOP", "Tonga Pa'anga", 2.17491));</v>
       </c>
       <c r="K164">
         <v>21495</v>
@@ -6047,11 +6197,12 @@
         <v>325</v>
       </c>
       <c r="C165">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>6.3381999999999996</v>
       </c>
       <c r="E165" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("TTD", "Trinidad/Tobago Dollar", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("TTD", "Trinidad/Tobago Dollar", 6.3382));</v>
       </c>
       <c r="K165">
         <v>114.485001</v>
@@ -6068,11 +6219,12 @@
         <v>326</v>
       </c>
       <c r="C166">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>1.9515499999999999</v>
       </c>
       <c r="E166" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("TND", "Tunisian Dinar", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("TND", "Tunisian Dinar", 1.95155));</v>
       </c>
       <c r="K166">
         <v>15.34</v>
@@ -6089,11 +6241,12 @@
         <v>671</v>
       </c>
       <c r="C167">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>3.0063499999999999</v>
       </c>
       <c r="E167" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("TRY", "Turkish Lira", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("TRY", "Turkish Lira", 3.00635));</v>
       </c>
       <c r="K167">
         <v>135.29499799999999</v>
@@ -6110,11 +6263,12 @@
         <v>328</v>
       </c>
       <c r="C168">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>3.5</v>
       </c>
       <c r="E168" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("TMT", "Turkmenistan Manat", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("TMT", "Turkmenistan Manat", 3.5));</v>
       </c>
       <c r="K168">
         <v>7.8304999999999998</v>
@@ -6131,11 +6285,12 @@
         <v>330</v>
       </c>
       <c r="C169">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>3650</v>
       </c>
       <c r="E169" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("UGX", "Uganda Shilling", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("UGX", "Uganda Shilling", 3650));</v>
       </c>
       <c r="K169">
         <v>3.6438000000000001</v>
@@ -6152,11 +6307,12 @@
         <v>672</v>
       </c>
       <c r="C170">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>21.799999</v>
       </c>
       <c r="E170" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("UAH", "Ukrainian Hryvnia", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("UAH", "Ukrainian Hryvnia", 21.799999));</v>
       </c>
       <c r="K170">
         <v>0.38505</v>
@@ -6173,11 +6329,12 @@
         <v>673</v>
       </c>
       <c r="C171">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>3.6727500000000002</v>
       </c>
       <c r="E171" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("AED", "United Arab Emirates Dirham", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("AED", "United Arab Emirates Dirham", 3.67275));</v>
       </c>
       <c r="K171">
         <v>97.049499999999995</v>
@@ -6194,11 +6351,12 @@
         <v>332</v>
       </c>
       <c r="C172">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>28.815000999999999</v>
       </c>
       <c r="E172" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("UYU", "Uruguayan Peso", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("UYU", "Uruguayan Peso", 28.815001));</v>
       </c>
       <c r="K172">
         <v>70.493797000000001</v>
@@ -6215,11 +6373,12 @@
         <v>354</v>
       </c>
       <c r="C173">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>2610.889893</v>
       </c>
       <c r="E173" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("UZS", "Uzbekistani Som", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("UZS", "Uzbekistani Som", 2610.889893));</v>
       </c>
       <c r="K173">
         <v>16.622399999999999</v>
@@ -6236,11 +6395,12 @@
         <v>334</v>
       </c>
       <c r="C174">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>114.485001</v>
       </c>
       <c r="E174" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("VUV", "Vanuatu Vatu", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("VUV", "Vanuatu Vatu", 114.485001));</v>
       </c>
       <c r="K174">
         <v>4.2264999999999997</v>
@@ -6257,11 +6417,12 @@
         <v>335</v>
       </c>
       <c r="C175">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>6.35</v>
       </c>
       <c r="E175" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("VEF", "Venezuelan Bolivar", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("VEF", "Venezuelan Bolivar", 6.35));</v>
       </c>
       <c r="K175">
         <v>207.21000699999999</v>
@@ -6278,11 +6439,12 @@
         <v>337</v>
       </c>
       <c r="C176">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>22475</v>
       </c>
       <c r="E176" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("VND", "Vietnamese Dong", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("VND", "Vietnamese Dong", 22475));</v>
       </c>
       <c r="K176">
         <v>13.315250000000001</v>
@@ -6299,11 +6461,12 @@
         <v>685</v>
       </c>
       <c r="C177">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>580.724243</v>
       </c>
       <c r="E177" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XOF", "West African CFA", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("XOF", "West African CFA", 580.724243));</v>
       </c>
       <c r="K177">
         <v>214.88999899999999</v>
@@ -6320,11 +6483,12 @@
         <v>338</v>
       </c>
       <c r="C178">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>214.88999899999999</v>
       </c>
       <c r="E178" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("YER", "Yemeni Rial", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("YER", "Yemeni Rial", 214.889999));</v>
       </c>
       <c r="K178">
         <v>3.7500499999999999</v>
@@ -6341,11 +6505,12 @@
         <v>339</v>
       </c>
       <c r="C179">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>10.003</v>
       </c>
       <c r="E179" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ZMW", "Zambian Kwacha", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ZMW", "Zambian Kwacha", 10.003));</v>
       </c>
       <c r="K179">
         <v>28.815000999999999</v>
@@ -6362,11 +6527,12 @@
         <v>708</v>
       </c>
       <c r="C180">
-        <v>1234</v>
+        <f t="shared" si="4"/>
+        <v>322.35501099999999</v>
       </c>
       <c r="E180" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ZWL", "Zimbabwean Dollar (obsolete)", 1234));</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  uc.addUnit(new UnitCurrency("ZWL", "Zimbabwean Dollar (obsolete)", 322.355011));</v>
       </c>
       <c r="K180">
         <v>0.64432999999999996</v>

</xml_diff>